<commit_message>
Changed to proper atomic names
</commit_message>
<xml_diff>
--- a/python_single_shooting/data.xlsx
+++ b/python_single_shooting/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karls\Dirac\ShootingDirac\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexa\Documents\Shooting_Dirac\python_single_shooting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC426F60-66CA-400A-B5CD-4A7D5AEE10FB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DC03B8C-1739-4692-96B5-BEED85E01243}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -85,27 +85,6 @@
     <t>40Ca 1f5/2</t>
   </si>
   <si>
-    <t>48Ca 1d5/2</t>
-  </si>
-  <si>
-    <t>48Ca 2s1/2</t>
-  </si>
-  <si>
-    <t>48Ca 1d3/2</t>
-  </si>
-  <si>
-    <t>48Ca 1f7/2</t>
-  </si>
-  <si>
-    <t>48Ca 2p3/2</t>
-  </si>
-  <si>
-    <t>48Ca 2p1/2</t>
-  </si>
-  <si>
-    <t>48Ca 1f5/2</t>
-  </si>
-  <si>
     <t>56Ni 1f7/2</t>
   </si>
   <si>
@@ -139,33 +118,6 @@
     <t>100Sn 2d3/2</t>
   </si>
   <si>
-    <t>132Sn 1g7/2</t>
-  </si>
-  <si>
-    <t>132Sn 2d5/2</t>
-  </si>
-  <si>
-    <t>132Sn 3s1/2</t>
-  </si>
-  <si>
-    <t>132Sn 1h11/2</t>
-  </si>
-  <si>
-    <t>132Sn 2d3/2</t>
-  </si>
-  <si>
-    <t>132Sn 2f7/2</t>
-  </si>
-  <si>
-    <t>132Sn 3p3/2</t>
-  </si>
-  <si>
-    <t>132Sn 1h9/2</t>
-  </si>
-  <si>
-    <t>132Sn 2f5/2</t>
-  </si>
-  <si>
     <t>208Pb 1h9/2</t>
   </si>
   <si>
@@ -211,12 +163,6 @@
     <t>100Sn 2p3/2</t>
   </si>
   <si>
-    <t>132Sn 2p1/2</t>
-  </si>
-  <si>
-    <t>132Sn 1g9/2</t>
-  </si>
-  <si>
     <t>208Pb 1g7/2</t>
   </si>
   <si>
@@ -236,6 +182,60 @@
   </si>
   <si>
     <t>a0_d</t>
+  </si>
+  <si>
+    <t>132Cs 1g7/2</t>
+  </si>
+  <si>
+    <t>132Cs 2d5/2</t>
+  </si>
+  <si>
+    <t>132Cs 2d3/2</t>
+  </si>
+  <si>
+    <t>132Cs 1h11/2</t>
+  </si>
+  <si>
+    <t>132Cs 3s1/2</t>
+  </si>
+  <si>
+    <t>132Cs 2f7/2</t>
+  </si>
+  <si>
+    <t>132Cs 3p3/2</t>
+  </si>
+  <si>
+    <t>132Cs 1h9/2</t>
+  </si>
+  <si>
+    <t>132Cs 2f5/2</t>
+  </si>
+  <si>
+    <t>132Cs 2p1/2</t>
+  </si>
+  <si>
+    <t>132Cs 1g9/2</t>
+  </si>
+  <si>
+    <t>48Cd 1d5/2</t>
+  </si>
+  <si>
+    <t>48Cd 2s1/2</t>
+  </si>
+  <si>
+    <t>48Cd 1d3/2</t>
+  </si>
+  <si>
+    <t>48Cd 1f7/2</t>
+  </si>
+  <si>
+    <t>48Cd 2p3/2</t>
+  </si>
+  <si>
+    <t>48Cd 2p1/2</t>
+  </si>
+  <si>
+    <t>48Cd 1f5/2</t>
   </si>
 </sst>
 </file>
@@ -601,8 +601,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L90"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="O62" sqref="O62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -646,7 +646,7 @@
         <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>71</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -1034,7 +1034,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>65</v>
       </c>
       <c r="C12">
         <v>-1</v>
@@ -1072,7 +1072,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>22</v>
+        <v>66</v>
       </c>
       <c r="C13">
         <v>-1</v>
@@ -1110,7 +1110,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>23</v>
+        <v>67</v>
       </c>
       <c r="C14">
         <v>-1</v>
@@ -1148,7 +1148,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>24</v>
+        <v>68</v>
       </c>
       <c r="C15">
         <v>-1</v>
@@ -1186,7 +1186,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>25</v>
+        <v>69</v>
       </c>
       <c r="C16">
         <v>-1</v>
@@ -1224,7 +1224,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>26</v>
+        <v>70</v>
       </c>
       <c r="C17">
         <v>-1</v>
@@ -1262,7 +1262,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>27</v>
+        <v>71</v>
       </c>
       <c r="C18">
         <v>-1</v>
@@ -1300,7 +1300,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C19">
         <v>-1</v>
@@ -1338,7 +1338,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="C20">
         <v>-1</v>
@@ -1376,7 +1376,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C21">
         <v>-1</v>
@@ -1414,7 +1414,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C22">
         <v>-1</v>
@@ -1452,7 +1452,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="C23">
         <v>-1</v>
@@ -1490,7 +1490,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C24">
         <v>-1</v>
@@ -1528,7 +1528,7 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C25">
         <v>-1</v>
@@ -1566,7 +1566,7 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="C26">
         <v>-1</v>
@@ -1604,7 +1604,7 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C27">
         <v>-1</v>
@@ -1642,7 +1642,7 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C28">
         <v>-1</v>
@@ -1680,7 +1680,7 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C29">
         <v>-1</v>
@@ -1718,7 +1718,7 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="C30">
         <v>-1</v>
@@ -1756,7 +1756,7 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="C31">
         <v>-1</v>
@@ -1794,7 +1794,7 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="C32">
         <v>-1</v>
@@ -1832,7 +1832,7 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="C33">
         <v>-1</v>
@@ -1870,7 +1870,7 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="C34">
         <v>-1</v>
@@ -1908,7 +1908,7 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="C35">
         <v>-1</v>
@@ -1946,7 +1946,7 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="C36">
         <v>-1</v>
@@ -1984,7 +1984,7 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="C37">
         <v>-1</v>
@@ -2022,7 +2022,7 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="C38">
         <v>-1</v>
@@ -2060,7 +2060,7 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="C39">
         <v>-1</v>
@@ -2098,7 +2098,7 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="C40">
         <v>-1</v>
@@ -2136,7 +2136,7 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="C41">
         <v>-1</v>
@@ -2174,7 +2174,7 @@
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="C42">
         <v>-1</v>
@@ -2212,7 +2212,7 @@
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="C43">
         <v>-1</v>
@@ -2250,7 +2250,7 @@
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="C44">
         <v>-1</v>
@@ -2288,7 +2288,7 @@
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="C45">
         <v>-1</v>
@@ -2326,7 +2326,7 @@
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="C46">
         <v>-1</v>
@@ -2364,7 +2364,7 @@
         <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="C47">
         <v>-1</v>
@@ -2402,7 +2402,7 @@
         <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="C48">
         <v>-1</v>
@@ -2440,7 +2440,7 @@
         <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="C49">
         <v>-1</v>
@@ -2478,7 +2478,7 @@
         <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="C50">
         <v>-1</v>
@@ -2630,7 +2630,7 @@
         <v>52</v>
       </c>
       <c r="B54" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="C54">
         <v>1</v>
@@ -2858,7 +2858,7 @@
         <v>58</v>
       </c>
       <c r="B60" t="s">
-        <v>21</v>
+        <v>65</v>
       </c>
       <c r="C60">
         <v>1</v>
@@ -2896,7 +2896,7 @@
         <v>59</v>
       </c>
       <c r="B61" t="s">
-        <v>23</v>
+        <v>67</v>
       </c>
       <c r="C61">
         <v>1</v>
@@ -2934,7 +2934,7 @@
         <v>60</v>
       </c>
       <c r="B62" t="s">
-        <v>22</v>
+        <v>66</v>
       </c>
       <c r="C62">
         <v>1</v>
@@ -2972,7 +2972,7 @@
         <v>61</v>
       </c>
       <c r="B63" t="s">
-        <v>24</v>
+        <v>68</v>
       </c>
       <c r="C63">
         <v>1</v>
@@ -3010,7 +3010,7 @@
         <v>62</v>
       </c>
       <c r="B64" t="s">
-        <v>25</v>
+        <v>69</v>
       </c>
       <c r="C64">
         <v>1</v>
@@ -3048,7 +3048,7 @@
         <v>63</v>
       </c>
       <c r="B65" t="s">
-        <v>26</v>
+        <v>70</v>
       </c>
       <c r="C65">
         <v>1</v>
@@ -3086,7 +3086,7 @@
         <v>64</v>
       </c>
       <c r="B66" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C66">
         <v>1</v>
@@ -3124,7 +3124,7 @@
         <v>65</v>
       </c>
       <c r="B67" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="C67">
         <v>1</v>
@@ -3162,7 +3162,7 @@
         <v>66</v>
       </c>
       <c r="B68" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C68">
         <v>1</v>
@@ -3200,7 +3200,7 @@
         <v>67</v>
       </c>
       <c r="B69" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C69">
         <v>1</v>
@@ -3238,7 +3238,7 @@
         <v>68</v>
       </c>
       <c r="B70" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="C70">
         <v>1</v>
@@ -3276,7 +3276,7 @@
         <v>69</v>
       </c>
       <c r="B71" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="C71">
         <v>1</v>
@@ -3314,7 +3314,7 @@
         <v>70</v>
       </c>
       <c r="B72" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="C72">
         <v>1</v>
@@ -3352,7 +3352,7 @@
         <v>71</v>
       </c>
       <c r="B73" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C73">
         <v>1</v>
@@ -3390,7 +3390,7 @@
         <v>72</v>
       </c>
       <c r="B74" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="C74">
         <v>1</v>
@@ -3504,7 +3504,7 @@
         <v>75</v>
       </c>
       <c r="B77" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="C77">
         <v>1</v>
@@ -3542,7 +3542,7 @@
         <v>76</v>
       </c>
       <c r="B78" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="C78">
         <v>1</v>
@@ -3580,7 +3580,7 @@
         <v>77</v>
       </c>
       <c r="B79" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="C79">
         <v>1</v>
@@ -3618,7 +3618,7 @@
         <v>78</v>
       </c>
       <c r="B80" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="C80">
         <v>1</v>
@@ -3656,7 +3656,7 @@
         <v>79</v>
       </c>
       <c r="B81" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="C81">
         <v>1</v>
@@ -3694,7 +3694,7 @@
         <v>80</v>
       </c>
       <c r="B82" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="C82">
         <v>1</v>
@@ -3732,7 +3732,7 @@
         <v>81</v>
       </c>
       <c r="B83" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
       <c r="C83">
         <v>1</v>
@@ -3770,7 +3770,7 @@
         <v>82</v>
       </c>
       <c r="B84" t="s">
-        <v>68</v>
+        <v>50</v>
       </c>
       <c r="C84">
         <v>1</v>
@@ -3808,7 +3808,7 @@
         <v>83</v>
       </c>
       <c r="B85" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
       <c r="C85">
         <v>1</v>
@@ -3846,7 +3846,7 @@
         <v>84</v>
       </c>
       <c r="B86" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="C86">
         <v>1</v>
@@ -3884,7 +3884,7 @@
         <v>85</v>
       </c>
       <c r="B87" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="C87">
         <v>1</v>
@@ -3922,7 +3922,7 @@
         <v>86</v>
       </c>
       <c r="B88" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="C88">
         <v>1</v>
@@ -3960,7 +3960,7 @@
         <v>87</v>
       </c>
       <c r="B89" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="C89">
         <v>1</v>
@@ -3998,7 +3998,7 @@
         <v>88</v>
       </c>
       <c r="B90" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="C90">
         <v>1</v>

</xml_diff>